<commit_message>
feat: added persistent browser
</commit_message>
<xml_diff>
--- a/applications.xlsx
+++ b/applications.xlsx
@@ -606,7 +606,7 @@
         <v>2025-05-12T20:30:39.693185+00:00</v>
       </c>
       <c r="D3" t="str">
-        <v>2025-05-19T06:10:47.297+00:00</v>
+        <v>2025-05-21T05:27:16.484+00:00</v>
       </c>
       <c r="E3" t="str">
         <v>Software Engineer</v>
@@ -666,7 +666,7 @@
         <v>hello</v>
       </c>
       <c r="X3" t="str">
-        <v>Hello world</v>
+        <v>Hello world, trust you are all good right?</v>
       </c>
       <c r="Y3" t="str">
         <v/>

</xml_diff>